<commit_message>
Zaktualizwana struktura ramki, dodany znak końca
</commit_message>
<xml_diff>
--- a/ramka.xlsx
+++ b/ramka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\wlasny_protokol_komunikacyjny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6BC1A8-0F0C-470F-9C4D-542249003AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78160CB1-D293-4047-8092-67795724D94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{7CA8A3FD-EFCD-4D03-8A3D-6423114218DD}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>0-7</t>
   </si>
@@ -190,13 +190,19 @@
   </si>
   <si>
     <t xml:space="preserve"> - suma kontrolna pola danych</t>
+  </si>
+  <si>
+    <t>END_BIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - bit końca ramki '\n'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,13 +225,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="6">
@@ -653,9 +652,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -665,34 +661,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,33 +682,66 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1072,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BCCE65-6784-4462-840B-B439189A954F}">
-  <dimension ref="A3:K34"/>
+  <dimension ref="A3:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:K30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1086,10 +1087,10 @@
   <sheetData>
     <row r="3" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1113,45 +1114,45 @@
       <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="38" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="10"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1163,387 +1164,435 @@
       <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="32"/>
       <c r="H6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="13"/>
-      <c r="K7" s="10"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="8" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15" t="s">
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18" t="s">
+      <c r="G8" s="42"/>
+      <c r="H8" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="I8" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="40"/>
     </row>
     <row r="10" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="11" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="37"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="38"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="39"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="38"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
     </row>
     <row r="14" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="38"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="39"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="38"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="41"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="25"/>
     </row>
     <row r="16" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="38"/>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="39"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="31"/>
     </row>
     <row r="17" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="38"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="41"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="25"/>
     </row>
     <row r="18" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="38"/>
-      <c r="C18" s="20" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="39"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31"/>
     </row>
     <row r="19" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="38"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="41"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="25"/>
     </row>
     <row r="20" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="38"/>
-      <c r="C20" s="21" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="39"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="31"/>
     </row>
     <row r="21" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="38"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="41"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="25"/>
     </row>
     <row r="22" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="38"/>
-      <c r="C22" s="19" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="39"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="31"/>
     </row>
     <row r="23" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="38"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="41"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="25"/>
     </row>
     <row r="24" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="38"/>
-      <c r="C24" s="19" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="39"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="31"/>
     </row>
     <row r="25" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="44"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="28"/>
     </row>
     <row r="26" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B26" s="38"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40"/>
-      <c r="K26" s="41"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
     </row>
     <row r="27" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="38"/>
-      <c r="C27" s="22" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="39"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="31"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B28" s="38"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="41"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="25"/>
     </row>
     <row r="29" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="38"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="41"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="25"/>
     </row>
     <row r="30" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="38"/>
-      <c r="C30" s="23" t="s">
+      <c r="B30" s="23"/>
+      <c r="C30" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="39"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="31"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B31" s="38"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="41"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="25"/>
     </row>
     <row r="32" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="38"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="41"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="25"/>
     </row>
     <row r="33" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="38"/>
-      <c r="C33" s="24" t="s">
+      <c r="B33" s="23"/>
+      <c r="C33" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="39"/>
-    </row>
-    <row r="34" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="44"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B34" s="23"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="25"/>
+    </row>
+    <row r="35" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="25"/>
+    </row>
+    <row r="36" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B36" s="23"/>
+      <c r="C36" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="K4:K8"/>
+    <mergeCell ref="F8:G8"/>
     <mergeCell ref="D27:K27"/>
     <mergeCell ref="D30:K30"/>
     <mergeCell ref="D33:K33"/>
@@ -1554,11 +1603,6 @@
     <mergeCell ref="D20:K20"/>
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D24:K24"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="K4:K8"/>
-    <mergeCell ref="F8:H8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>